<commit_message>
added a few code changes for confusion matrix
</commit_message>
<xml_diff>
--- a/Result_data/DE_SVM_10_6.xlsx
+++ b/Result_data/DE_SVM_10_6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="28">
   <si>
     <t>precision</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>DE SVM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local learning + hyper parameter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">screen dump of stack over flow on 1st few page </t>
+  </si>
+  <si>
+    <t>Defect Prediction and Class Imbalance</t>
   </si>
 </sst>
 </file>
@@ -7601,8 +7610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABD84A7-1C89-4823-974D-3BC2866F14C4}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:C61"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8378,18 +8387,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD57A980-855F-4620-BC0C-775DF77023E3}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -8403,7 +8413,7 @@
         <v>21907.180684522398</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -8417,7 +8427,7 @@
         <v>22152.939994333799</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D3">
         <f>SUM(D1:D2)</f>
         <v>44060.120678856198</v>
@@ -8427,10 +8437,32 @@
         <v>12.238922410793387</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5">
         <f>D3/60</f>
         <v>734.33534464760328</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <f>D5*E5</f>
+        <v>73433.534464760334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>